<commit_message>
corercted session notes method type
</commit_message>
<xml_diff>
--- a/SessionNotes_PartA.xlsx
+++ b/SessionNotes_PartA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wwang\OneDrive\Desktop\MCGILL\FALL 2024\ECSE 429\Project\Part1\GitHub\ECSE429_Project_PartA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{636A4019-C4BA-486F-9705-B8559ABF9579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17BAB5ED-3A3C-48F6-A12D-99720500E7C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes Session 1" sheetId="1" r:id="rId1"/>
@@ -543,7 +543,18 @@
     <cellStyle name="Accent2" xfId="1" builtinId="33"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="64">
+  <dxfs count="59">
+    <dxf>
+      <font>
+        <color rgb="FF7F7F7F"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7F7F7F"/>
+          <bgColor rgb="FF7F7F7F"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -586,6 +597,47 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFAD00"/>
+          <bgColor rgb="FFFFAD00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00B050"/>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFAD00"/>
+          <bgColor rgb="FFFFAD00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -604,6 +656,14 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFC6EFCE"/>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFAD00"/>
+          <bgColor rgb="FFFFAD00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -663,106 +723,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFB764FF"/>
           <bgColor rgb="FFB764FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFAD00"/>
-          <bgColor rgb="FFFFAD00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFAD00"/>
-          <bgColor rgb="FFFFAD00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFAD00"/>
-          <bgColor rgb="FFFFAD00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFAD00"/>
-          <bgColor rgb="FFFFAD00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFAD00"/>
-          <bgColor rgb="FFFFAD00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFAD00"/>
-          <bgColor rgb="FFFFAD00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFAD00"/>
-          <bgColor rgb="FFFFAD00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7F7F7F"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7F7F7F"/>
-          <bgColor rgb="FF7F7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00B050"/>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFAD00"/>
-          <bgColor rgb="FFFFAD00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -901,23 +861,23 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFC6EFCE"/>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -935,8 +895,8 @@
       </font>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFFAD00"/>
-          <bgColor rgb="FFFFAD00"/>
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -957,8 +917,8 @@
       </font>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
+          <fgColor rgb="FFFFAD00"/>
+          <bgColor rgb="FFFFAD00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1001,42 +961,13 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFB764FF"/>
-          <bgColor rgb="FFB764FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF005B"/>
-          <bgColor rgb="FFFF005B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC000"/>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
+          <fgColor rgb="FF00B0F0"/>
+          <bgColor rgb="FF00B0F0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1049,35 +980,10 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF00B0F0"/>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1114,6 +1020,39 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00B0F0"/>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF00B050"/>
@@ -1130,13 +1069,34 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF00B0F0"/>
-          <bgColor rgb="FF00B0F0"/>
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF005B"/>
+          <bgColor rgb="FFFF005B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB764FF"/>
+          <bgColor rgb="FFB764FF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4771,119 +4731,119 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="B1:B14">
-    <cfRule type="cellIs" dxfId="63" priority="22" operator="equal">
-      <formula>"PUT"</formula>
+    <cfRule type="cellIs" dxfId="58" priority="16" operator="equal">
+      <formula>"PATCH"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="17" operator="equal">
+      <formula>"HEAD"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="56" priority="18" operator="equal">
+      <formula>"OPTIONS"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="55" priority="19" operator="equal">
+      <formula>"DELETE"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="20" operator="equal">
       <formula>"POST"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="21" operator="equal">
       <formula>"GET"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="16" operator="equal">
-      <formula>"PATCH"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="17" operator="equal">
-      <formula>"HEAD"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="18" operator="equal">
-      <formula>"OPTIONS"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="19" operator="equal">
-      <formula>"DELETE"</formula>
+    <cfRule type="cellIs" dxfId="52" priority="22" operator="equal">
+      <formula>"PUT"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C14">
-    <cfRule type="cellIs" dxfId="56" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="14" operator="equal">
       <formula>"DOCUMENTED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="15" operator="equal">
       <formula>"UNDOCUMENTED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:C17 C19:C25 C27:C33 C35:C41 C43:C1000">
-    <cfRule type="cellIs" dxfId="54" priority="55" operator="equal">
-      <formula>"PUT"</formula>
+    <cfRule type="cellIs" dxfId="49" priority="49" operator="equal">
+      <formula>"PATCH"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="50" operator="equal">
+      <formula>"HEAD"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="47" priority="51" operator="equal">
+      <formula>"OPTIONS"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="52" operator="equal">
+      <formula>"DELETE"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="45" priority="53" operator="equal">
+      <formula>"POST"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="54" operator="equal">
       <formula>"GET"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="53" operator="equal">
-      <formula>"POST"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="52" operator="equal">
-      <formula>"DELETE"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="51" operator="equal">
-      <formula>"OPTIONS"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="50" operator="equal">
-      <formula>"HEAD"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="49" operator="equal">
-      <formula>"PATCH"</formula>
+    <cfRule type="cellIs" dxfId="43" priority="55" operator="equal">
+      <formula>"PUT"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D11 E15:E17 E19:E25 E27:E33 E35:E41 E43:E49">
-    <cfRule type="cellIs" dxfId="47" priority="62" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="62" stopIfTrue="1" operator="equal">
       <formula>"method not allowed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12 D15:D17 D19:D25 D27:D33 D35:D41 D43:D1000">
-    <cfRule type="cellIs" dxfId="46" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="56" operator="equal">
       <formula>"DOCUMENTED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="57" operator="equal">
       <formula>"UNDOCUMENTED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13:D14">
-    <cfRule type="cellIs" dxfId="44" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="2" stopIfTrue="1" operator="equal">
       <formula>"method not allowed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E14">
-    <cfRule type="cellIs" dxfId="43" priority="13" operator="equal">
-      <formula>"NO"</formula>
+    <cfRule type="cellIs" dxfId="38" priority="11" operator="equal">
+      <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="12" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="11" operator="equal">
-      <formula>"N/A"</formula>
+    <cfRule type="cellIs" dxfId="36" priority="13" operator="equal">
+      <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10:F11">
-    <cfRule type="cellIs" dxfId="40" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="4" stopIfTrue="1" operator="equal">
       <formula>"method not allowed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12">
-    <cfRule type="cellIs" dxfId="39" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="6" operator="equal">
+      <formula>"DOCUMENTED"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="7" operator="equal">
       <formula>"UNDOCUMENTED"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="6" operator="equal">
-      <formula>"DOCUMENTED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14">
-    <cfRule type="cellIs" dxfId="37" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="1" stopIfTrue="1" operator="equal">
       <formula>"method not allowed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15:F17 F19:F25 F27:F33 F35:F41 F43:F1000">
-    <cfRule type="cellIs" dxfId="36" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="58" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="59" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="60" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G11 G13 G15:G17 G19:G25 G27:G33 G35:G41 G43:G49">
-    <cfRule type="expression" dxfId="33" priority="61">
+    <cfRule type="expression" dxfId="28" priority="61">
       <formula>$E11="method not allowed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5239,8 +5199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D412421-5CA2-4299-9F7F-6CA1BD717DAE}">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15" customHeight="1"/>
@@ -5432,7 +5392,7 @@
         <v>33</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>5</v>
@@ -5456,7 +5416,7 @@
         <v>33</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>5</v>
@@ -7914,122 +7874,107 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <conditionalFormatting sqref="B1:B11">
-    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="8" operator="equal">
       <formula>"PATCH"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="9" operator="equal">
       <formula>"HEAD"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="10" operator="equal">
       <formula>"OPTIONS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="11" operator="equal">
       <formula>"DELETE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="12" operator="equal">
       <formula>"POST"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="13" operator="equal">
       <formula>"GET"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="14" operator="equal">
       <formula>"PUT"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C11">
-    <cfRule type="cellIs" dxfId="5" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="15" operator="equal">
       <formula>"DOCUMENTED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="16" operator="equal">
       <formula>"UNDOCUMENTED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:C17 C19:C25 C27:C33 C35:C41 C43:C1000">
-    <cfRule type="cellIs" dxfId="32" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
       <formula>"PATCH"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="21" operator="equal">
       <formula>"HEAD"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="22" operator="equal">
       <formula>"OPTIONS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="23" operator="equal">
       <formula>"DELETE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="24" operator="equal">
       <formula>"POST"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="25" operator="equal">
       <formula>"GET"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="26" operator="equal">
       <formula>"PUT"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E12:E17 E19:E25 E27:E33 E35:E41 E43:E49 D2:D11">
-    <cfRule type="cellIs" dxfId="3" priority="33" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="D2:D11 E12:E17 E19:E25 E27:E33 E35:E41 E43:E49">
+    <cfRule type="cellIs" dxfId="11" priority="33" stopIfTrue="1" operator="equal">
       <formula>"method not allowed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12:D17 D19:D25 D27:D33 D35:D41 D43:D1000">
-    <cfRule type="cellIs" dxfId="25" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="27" operator="equal">
       <formula>"DOCUMENTED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="28" operator="equal">
       <formula>"UNDOCUMENTED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E11">
-    <cfRule type="cellIs" dxfId="2" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="17" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="18" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="19" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="F3">
+    <cfRule type="cellIs" dxfId="5" priority="1" stopIfTrue="1" operator="equal">
+      <formula>"method not allowed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8:F11">
+    <cfRule type="cellIs" dxfId="4" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"method not allowed"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F12:F17 F19:F25 F27:F33 F35:F41 F43:F1000">
-    <cfRule type="cellIs" dxfId="23" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="29" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="30" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="31" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12:G17 G19:G25 G27:G33 G35:G41 G43:G49">
-    <cfRule type="expression" dxfId="20" priority="32">
+    <cfRule type="expression" dxfId="0" priority="32">
       <formula>$E12="method not allowed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F9">
-    <cfRule type="cellIs" dxfId="17" priority="5" stopIfTrue="1" operator="equal">
-      <formula>"method not allowed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="16" priority="4" stopIfTrue="1" operator="equal">
-      <formula>"method not allowed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F11">
-    <cfRule type="cellIs" dxfId="15" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"method not allowed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F10">
-    <cfRule type="cellIs" dxfId="14" priority="2" stopIfTrue="1" operator="equal">
-      <formula>"method not allowed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F3">
-    <cfRule type="cellIs" dxfId="13" priority="1" stopIfTrue="1" operator="equal">
-      <formula>"method not allowed"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
@@ -8059,7 +8004,7 @@
   </sheetPr>
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>

</xml_diff>